<commit_message>
PGN233 Tool Data fixed
</commit_message>
<xml_diff>
--- a/SourceCode/AOG/PGN 9.xlsx
+++ b/SourceCode/AOG/PGN 9.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="233">
   <si>
     <t xml:space="preserve">PGN Name</t>
   </si>
@@ -490,19 +490,16 @@
     <t xml:space="preserve">E9</t>
   </si>
   <si>
-    <t xml:space="preserve">Low XTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High XTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low Veh XTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Veh XTE</t>
+    <t xml:space="preserve">Tool XTE (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle XTE (mm)</t>
   </si>
   <si>
     <t xml:space="preserve">Speed * 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Heading Deg * 10</t>
   </si>
   <si>
     <t xml:space="preserve">IP = 192.168.5.226</t>
@@ -1044,7 +1041,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1306,10 +1303,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1609,7 +1602,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
+      <selection pane="bottomLeft" activeCell="R60" activeCellId="0" sqref="R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3274,27 +3267,21 @@
       <c r="I58" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="J58" s="23" t="s">
-        <v>156</v>
-      </c>
+      <c r="J58" s="62"/>
       <c r="K58" s="23" t="s">
         <v>20</v>
       </c>
       <c r="L58" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="M58" s="23"/>
+      <c r="N58" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="M58" s="23" t="s">
+      <c r="O58" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="N58" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="O58" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="P58" s="23" t="s">
-        <v>57</v>
-      </c>
+      <c r="P58" s="23"/>
       <c r="Q58" s="23" t="s">
         <v>25</v>
       </c>
@@ -3328,16 +3315,16 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G60" s="7" t="n">
         <v>232</v>
@@ -3346,10 +3333,10 @@
         <v>8</v>
       </c>
       <c r="I60" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J60" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="J60" s="10" t="s">
-        <v>164</v>
       </c>
       <c r="K60" s="10" t="s">
         <v>32</v>
@@ -3358,16 +3345,16 @@
         <v>30</v>
       </c>
       <c r="M60" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="N60" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="N60" s="66" t="s">
+      <c r="O60" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="O60" s="10" t="s">
+      <c r="P60" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="P60" s="10" t="s">
-        <v>168</v>
       </c>
       <c r="Q60" s="10" t="s">
         <v>25</v>
@@ -3376,7 +3363,7 @@
     <row r="61" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
       <c r="B61" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="4"/>
@@ -3422,17 +3409,17 @@
     <row r="62" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
       <c r="B62" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G62" s="7" t="n">
         <v>231</v>
@@ -3441,16 +3428,16 @@
         <v>8</v>
       </c>
       <c r="I62" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="J62" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="K62" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="K62" s="10" t="s">
+      <c r="L62" s="10" t="s">
         <v>175</v>
-      </c>
-      <c r="L62" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="M62" s="10" t="s">
         <v>57</v>
@@ -3496,7 +3483,7 @@
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="54"/>
       <c r="B63" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J63" s="1"/>
       <c r="L63" s="1"/>
@@ -3530,16 +3517,16 @@
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="C64" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>122</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G64" s="7" t="n">
         <v>230</v>
@@ -3548,19 +3535,19 @@
         <v>8</v>
       </c>
       <c r="I64" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="J64" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="J64" s="8" t="s">
+      <c r="K64" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="K64" s="8" t="s">
+      <c r="L64" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="L64" s="8" t="s">
+      <c r="M64" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="M64" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="N64" s="8" t="s">
         <v>20</v>
@@ -3646,7 +3633,7 @@
     </row>
     <row r="66" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="55"/>
-      <c r="B66" s="67"/>
+      <c r="B66" s="66"/>
       <c r="C66" s="57"/>
       <c r="D66" s="58"/>
       <c r="E66" s="59"/>
@@ -3692,7 +3679,7 @@
       <c r="A67" s="54"/>
       <c r="B67" s="25"/>
       <c r="C67" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D67" s="4" t="n">
         <v>77</v>
@@ -3701,35 +3688,35 @@
         <v>119</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G67" s="7" t="n">
         <v>234</v>
       </c>
       <c r="H67" s="8"/>
       <c r="I67" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="J67" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="J67" s="8" t="s">
+      <c r="K67" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="L67" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="K67" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="L67" s="8" t="s">
+      <c r="M67" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="M67" s="8" t="s">
+      <c r="N67" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="N67" s="8" t="s">
+      <c r="O67" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="O67" s="8" t="s">
+      <c r="P67" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="P67" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="Q67" s="8" t="s">
         <v>25</v>
@@ -3888,10 +3875,10 @@
     </row>
     <row r="71" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>17</v>
@@ -3905,7 +3892,7 @@
         <v>3</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J71" s="8" t="n">
         <v>0</v>
@@ -3946,7 +3933,7 @@
       <c r="AN71" s="8"/>
     </row>
     <row r="72" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="68"/>
+      <c r="B72" s="67"/>
       <c r="C72" s="3"/>
       <c r="D72" s="4"/>
       <c r="E72" s="5"/>
@@ -3988,10 +3975,10 @@
     </row>
     <row r="73" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="D73" s="4" t="n">
         <v>126</v>
@@ -4005,19 +3992,19 @@
         <v>5</v>
       </c>
       <c r="I73" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="J73" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="J73" s="8" t="s">
+      <c r="K73" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="K73" s="8" t="s">
+      <c r="L73" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="L73" s="8" t="s">
+      <c r="M73" s="8" t="s">
         <v>203</v>
-      </c>
-      <c r="M73" s="8" t="s">
-        <v>204</v>
       </c>
       <c r="N73" s="8" t="s">
         <v>25</v>
@@ -4050,9 +4037,9 @@
       <c r="AN73" s="8"/>
     </row>
     <row r="74" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="68"/>
+      <c r="B74" s="67"/>
       <c r="C74" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D74" s="4" t="n">
         <v>123</v>
@@ -4066,10 +4053,10 @@
         <v>5</v>
       </c>
       <c r="I74" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="J74" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="K74" s="8" t="s">
         <v>57</v>
@@ -4111,9 +4098,9 @@
       <c r="AN74" s="8"/>
     </row>
     <row r="75" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="68"/>
+      <c r="B75" s="67"/>
       <c r="C75" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D75" s="4" t="n">
         <v>121</v>
@@ -4172,9 +4159,9 @@
       <c r="AN75" s="8"/>
     </row>
     <row r="76" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="68"/>
+      <c r="B76" s="67"/>
       <c r="C76" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D76" s="4" t="n">
         <v>120</v>
@@ -4275,10 +4262,10 @@
     </row>
     <row r="78" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>17</v>
@@ -4298,13 +4285,13 @@
         <v>201</v>
       </c>
       <c r="K78" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="L78" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="L78" s="8" t="s">
+      <c r="M78" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="M78" s="8" t="s">
-        <v>214</v>
       </c>
       <c r="N78" s="8" t="s">
         <v>25</v>
@@ -4379,10 +4366,10 @@
     </row>
     <row r="80" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="C80" s="69" t="s">
-        <v>215</v>
+        <v>209</v>
+      </c>
+      <c r="C80" s="68" t="s">
+        <v>214</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>17</v>
@@ -4438,7 +4425,7 @@
     </row>
     <row r="81" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="25"/>
-      <c r="C81" s="69"/>
+      <c r="C81" s="68"/>
       <c r="D81" s="4"/>
       <c r="E81" s="5"/>
       <c r="F81" s="6"/>
@@ -4479,12 +4466,12 @@
     </row>
     <row r="82" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D82" s="70" t="n">
+      <c r="D82" s="69" t="n">
         <v>126</v>
       </c>
       <c r="E82" s="5"/>
@@ -4496,25 +4483,25 @@
         <v>7</v>
       </c>
       <c r="I82" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J82" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="J82" s="8" t="s">
+      <c r="K82" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="K82" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="L82" s="8" t="n">
         <v>126</v>
       </c>
       <c r="M82" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="N82" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="N82" s="8" t="s">
+      <c r="O82" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="O82" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="P82" s="8" t="s">
         <v>25</v>
@@ -4547,9 +4534,9 @@
     <row r="83" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="25"/>
       <c r="C83" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D83" s="70" t="n">
+        <v>223</v>
+      </c>
+      <c r="D83" s="69" t="n">
         <v>123</v>
       </c>
       <c r="E83" s="5"/>
@@ -4561,25 +4548,25 @@
         <v>7</v>
       </c>
       <c r="I83" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J83" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="J83" s="8" t="s">
+      <c r="K83" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="K83" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="L83" s="8" t="n">
         <v>123</v>
       </c>
       <c r="M83" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="N83" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="N83" s="8" t="s">
+      <c r="O83" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="O83" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="P83" s="8" t="s">
         <v>25</v>
@@ -4612,9 +4599,9 @@
     <row r="84" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="25"/>
       <c r="C84" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D84" s="70" t="n">
+        <v>224</v>
+      </c>
+      <c r="D84" s="69" t="n">
         <v>121</v>
       </c>
       <c r="E84" s="5"/>
@@ -4626,25 +4613,25 @@
         <v>7</v>
       </c>
       <c r="I84" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J84" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="J84" s="8" t="s">
+      <c r="K84" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="K84" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="L84" s="8" t="n">
         <v>121</v>
       </c>
       <c r="M84" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="N84" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="N84" s="8" t="s">
+      <c r="O84" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="O84" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="P84" s="8" t="s">
         <v>25</v>
@@ -4678,9 +4665,9 @@
       <c r="A85" s="54"/>
       <c r="B85" s="25"/>
       <c r="C85" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D85" s="70" t="n">
+        <v>225</v>
+      </c>
+      <c r="D85" s="69" t="n">
         <v>120</v>
       </c>
       <c r="G85" s="7" t="n">
@@ -4690,25 +4677,25 @@
         <v>7</v>
       </c>
       <c r="I85" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J85" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="J85" s="8" t="s">
+      <c r="K85" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="K85" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="L85" s="8" t="n">
         <v>120</v>
       </c>
       <c r="M85" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="N85" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="N85" s="8" t="s">
+      <c r="O85" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="O85" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="P85" s="8" t="s">
         <v>25</v>
@@ -4743,7 +4730,7 @@
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="54"/>
       <c r="B86" s="25"/>
-      <c r="D86" s="70"/>
+      <c r="D86" s="69"/>
       <c r="J86" s="8"/>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
@@ -4780,24 +4767,24 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="71" t="s">
+      <c r="C88" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="D88" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="D88" s="72" t="s">
+      <c r="E88" s="72"/>
+      <c r="F88" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="E88" s="73"/>
-      <c r="F88" s="74" t="s">
+      <c r="G88" s="51"/>
+    </row>
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="75" t="s">
         <v>229</v>
-      </c>
-      <c r="G88" s="51"/>
-    </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C89" s="76" t="s">
-        <v>230</v>
       </c>
       <c r="D89" s="4" t="n">
         <v>254</v>
@@ -4813,15 +4800,15 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="75"/>
-      <c r="C90" s="76"/>
+      <c r="B90" s="74"/>
+      <c r="C90" s="75"/>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="75" t="s">
+      <c r="B91" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C91" s="76" t="s">
-        <v>231</v>
+      <c r="C91" s="75" t="s">
+        <v>230</v>
       </c>
       <c r="D91" s="4" t="n">
         <v>239</v>
@@ -4837,15 +4824,15 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="75"/>
-      <c r="C92" s="76"/>
+      <c r="B92" s="74"/>
+      <c r="C92" s="75"/>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="75" t="s">
+      <c r="B93" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C93" s="76" t="s">
-        <v>232</v>
+      <c r="C93" s="75" t="s">
+        <v>231</v>
       </c>
       <c r="F93" s="6" t="n">
         <v>211</v>
@@ -4855,22 +4842,22 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="75"/>
-      <c r="C94" s="76"/>
+      <c r="B94" s="74"/>
+      <c r="C94" s="75"/>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="75" t="s">
+      <c r="B95" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="C95" s="76" t="s">
-        <v>233</v>
+      <c r="C95" s="75" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N5:O5"/>
@@ -4880,6 +4867,9 @@
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="M30:N30"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="O58:P58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>